<commit_message>
Se modificó función para mostrar resultados.
</commit_message>
<xml_diff>
--- a/datosDePrueba.xlsx
+++ b/datosDePrueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daas0\Documents\Universidad\Semestre_6\Máquinas\proyectoMaquinas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C89AB4-8362-470C-B4C1-A432413360C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6724F471-AF39-451E-BE6C-79C854DC3F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{142D1487-5D05-4A1D-9FAA-0999597E1D26}"/>
+    <workbookView xWindow="7692" yWindow="444" windowWidth="11424" windowHeight="11796" xr2:uid="{142D1487-5D05-4A1D-9FAA-0999597E1D26}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>H</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>La</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>FlujoCentro</t>
   </si>
 </sst>
 </file>
@@ -442,7 +448,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC993DE7-57D7-4D73-8447-862C1450F2D9}">
-  <dimension ref="C7:G17"/>
+  <dimension ref="C7:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
@@ -453,7 +459,7 @@
     <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>1</v>
       </c>
@@ -467,7 +473,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>0.02</v>
       </c>
@@ -481,7 +487,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>0.2</v>
       </c>
@@ -495,7 +501,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>0.6</v>
       </c>
@@ -509,7 +515,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C11">
         <v>0.9</v>
       </c>
@@ -523,7 +529,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C12">
         <v>1.1000000000000001</v>
       </c>
@@ -537,7 +543,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>1.24</v>
       </c>
@@ -551,7 +557,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C14">
         <v>1.36</v>
       </c>
@@ -564,8 +570,11 @@
       <c r="G14">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="H14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C15">
         <v>1.45</v>
       </c>
@@ -579,12 +588,18 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C16">
         <v>1.51</v>
       </c>
       <c r="D16">
         <v>3000</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16">
+        <v>0.02</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.3">

</xml_diff>